<commit_message>
:truck: Ajout du planning du projet
</commit_message>
<xml_diff>
--- a/Planning du projet.xlsx
+++ b/Planning du projet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{765580E0-D616-4F09-9214-B56EFA294CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99227821-0D70-4891-AB13-555E24624AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1345,6 +1345,12 @@
     <xf numFmtId="169" fontId="11" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1356,12 +1362,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2021,107 +2021,107 @@
         <v>2</v>
       </c>
       <c r="B3" s="51"/>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="91">
+      <c r="D3" s="89"/>
+      <c r="E3" s="93">
         <f>DATE(2026, 2, 7)</f>
         <v>46060</v>
       </c>
-      <c r="F3" s="91"/>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="93"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="90">
         <f>I5</f>
         <v>46055</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="90">
         <f>P5</f>
         <v>46062</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="90">
         <f>W5</f>
         <v>46069</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="90">
         <f>AD5</f>
         <v>46076</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="90">
         <f>AK5</f>
         <v>46083</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="90">
         <f>AR5</f>
         <v>46090</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="90">
         <f>AY5</f>
         <v>46097</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="90">
         <f>BF5</f>
         <v>46104</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
@@ -4811,17 +4811,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D34">
     <cfRule type="dataBar" priority="14">
@@ -5019,15 +5019,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5315,6 +5306,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
@@ -5328,14 +5328,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5354,4 +5346,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>